<commit_message>
Update dropout excel sheets
</commit_message>
<xml_diff>
--- a/Training histories/Philipp/04 Experimenting with dropout/00_history_dropout_comparison.xlsx
+++ b/Training histories/Philipp/04 Experimenting with dropout/00_history_dropout_comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philippmetzger/Documents/GitHub/Deep_Learning_Project_Group_10/Training histories/Philipp/04 Experimenting with dropout/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205C6C0D-2402-4C49-866D-DD5D8A7F7430}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2BEBD54-ED51-5749-8AA4-84032D83904A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37300" yWindow="2860" windowWidth="28800" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33740" yWindow="3520" windowWidth="28800" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>val_acc_0_9</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>val_acc_0_7</t>
+  </si>
+  <si>
+    <t>val_acc_0_5</t>
   </si>
 </sst>
 </file>
@@ -255,7 +258,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-5F3E-3B41-BC00-F892D29EB895}"/>
+              <c16:uniqueId val="{00000000-50F2-F44D-838A-DAA230855211}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -342,7 +345,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-5F3E-3B41-BC00-F892D29EB895}"/>
+              <c16:uniqueId val="{00000001-50F2-F44D-838A-DAA230855211}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -429,7 +432,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-5F3E-3B41-BC00-F892D29EB895}"/>
+              <c16:uniqueId val="{00000002-50F2-F44D-838A-DAA230855211}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -442,7 +445,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>val_acc_0_7</c:v>
+                  <c:v>val_acc_0_5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -466,49 +469,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0.35697674751281738</c:v>
+                  <c:v>0.34069767594337458</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.48527130484580988</c:v>
+                  <c:v>0.4713178277015686</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.52364343404769897</c:v>
+                  <c:v>0.50736433267593384</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.53914725780487061</c:v>
+                  <c:v>0.53875970840454102</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.55271315574645996</c:v>
+                  <c:v>0.53217053413391113</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.56821703910827637</c:v>
+                  <c:v>0.57054263353347778</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.5728682279586792</c:v>
+                  <c:v>0.54767441749572754</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.56356590986251831</c:v>
+                  <c:v>0.56279069185256958</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.58720928430557251</c:v>
+                  <c:v>0.60775196552276611</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.58953487873077393</c:v>
+                  <c:v>0.58488374948501587</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.59573644399642944</c:v>
+                  <c:v>0.57984495162963867</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.59922480583190918</c:v>
+                  <c:v>0.60348838567733765</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.59069764614105225</c:v>
+                  <c:v>0.60348838567733765</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.58682173490524292</c:v>
+                  <c:v>0.60736435651779175</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.59108525514602661</c:v>
+                  <c:v>0.6003875732421875</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -516,7 +519,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-5F3E-3B41-BC00-F892D29EB895}"/>
+              <c16:uniqueId val="{00000003-50F2-F44D-838A-DAA230855211}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -529,7 +532,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>val_acc_0_9</c:v>
+                  <c:v>val_acc_0_7</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -553,49 +556,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0.29844960570335388</c:v>
+                  <c:v>0.35697674751281738</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.41589146852493292</c:v>
+                  <c:v>0.48527130484580988</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.44418603181838989</c:v>
+                  <c:v>0.52364343404769897</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.50348836183547974</c:v>
+                  <c:v>0.53914725780487061</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.51589149236679077</c:v>
+                  <c:v>0.55271315574645996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.55155038833618164</c:v>
+                  <c:v>0.56821703910827637</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.56279069185256958</c:v>
+                  <c:v>0.5728682279586792</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.53720933198928833</c:v>
+                  <c:v>0.56356590986251831</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.56550389528274536</c:v>
+                  <c:v>0.58720928430557251</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.5767441987991333</c:v>
+                  <c:v>0.58953487873077393</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.60116279125213623</c:v>
+                  <c:v>0.59573644399642944</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.59534883499145508</c:v>
+                  <c:v>0.59922480583190918</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.59457361698150635</c:v>
+                  <c:v>0.59069764614105225</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.60581398010253906</c:v>
+                  <c:v>0.58682173490524292</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.61356586217880249</c:v>
+                  <c:v>0.59108525514602661</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -603,7 +606,94 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-5F3E-3B41-BC00-F892D29EB895}"/>
+              <c16:uniqueId val="{00000004-50F2-F44D-838A-DAA230855211}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>val_acc_0_9</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.29844960570335388</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.41589146852493292</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.44418603181838989</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.50348836183547974</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.51589149236679077</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.55155038833618164</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.56279069185256958</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.53720933198928833</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.56550389528274536</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.5767441987991333</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.60116279125213623</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.59534883499145508</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.59457361698150635</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.60581398010253906</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.61356586217880249</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-50F2-F44D-838A-DAA230855211}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -616,11 +706,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="274666143"/>
-        <c:axId val="274608159"/>
+        <c:axId val="306336847"/>
+        <c:axId val="306283039"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="274666143"/>
+        <c:axId val="306336847"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -662,7 +752,7 @@
             <a:endParaRPr lang="en-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="274608159"/>
+        <c:crossAx val="306283039"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -670,7 +760,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="274608159"/>
+        <c:axId val="306283039"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -721,7 +811,7 @@
             <a:endParaRPr lang="en-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="274666143"/>
+        <c:crossAx val="306336847"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1369,22 +1459,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:colOff>82550</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>584200</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>88900</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C1EBEA4F-CD40-5E43-B2F8-83E9F9F00AA5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC14B871-A31A-BE45-800F-C1F25F3FD32F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1690,21 +1780,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F16"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.1640625" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1715,13 +1805,16 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1735,13 +1828,16 @@
         <v>0.35736432671546942</v>
       </c>
       <c r="E2">
+        <v>0.34069767594337458</v>
+      </c>
+      <c r="F2">
         <v>0.35697674751281738</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0.29844960570335388</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1755,13 +1851,16 @@
         <v>0.46085271239280701</v>
       </c>
       <c r="E3">
+        <v>0.4713178277015686</v>
+      </c>
+      <c r="F3">
         <v>0.48527130484580988</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.41589146852493292</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1775,13 +1874,16 @@
         <v>0.49069768190383911</v>
       </c>
       <c r="E4">
+        <v>0.50736433267593384</v>
+      </c>
+      <c r="F4">
         <v>0.52364343404769897</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0.44418603181838989</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1795,13 +1897,16 @@
         <v>0.51550388336181641</v>
       </c>
       <c r="E5">
+        <v>0.53875970840454102</v>
+      </c>
+      <c r="F5">
         <v>0.53914725780487061</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>0.50348836183547974</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1815,13 +1920,16 @@
         <v>0.53759688138961792</v>
       </c>
       <c r="E6">
+        <v>0.53217053413391113</v>
+      </c>
+      <c r="F6">
         <v>0.55271315574645996</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>0.51589149236679077</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1835,13 +1943,16 @@
         <v>0.52674418687820435</v>
       </c>
       <c r="E7">
+        <v>0.57054263353347778</v>
+      </c>
+      <c r="F7">
         <v>0.56821703910827637</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>0.55155038833618164</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1855,13 +1966,16 @@
         <v>0.53449612855911255</v>
       </c>
       <c r="E8">
+        <v>0.54767441749572754</v>
+      </c>
+      <c r="F8">
         <v>0.5728682279586792</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>0.56279069185256958</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1875,13 +1989,16 @@
         <v>0.54302322864532471</v>
       </c>
       <c r="E9">
+        <v>0.56279069185256958</v>
+      </c>
+      <c r="F9">
         <v>0.56356590986251831</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>0.53720933198928833</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1895,13 +2012,16 @@
         <v>0.54844963550567627</v>
       </c>
       <c r="E10">
+        <v>0.60775196552276611</v>
+      </c>
+      <c r="F10">
         <v>0.58720928430557251</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>0.56550389528274536</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1915,13 +2035,16 @@
         <v>0.57131785154342651</v>
       </c>
       <c r="E11">
+        <v>0.58488374948501587</v>
+      </c>
+      <c r="F11">
         <v>0.58953487873077393</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>0.5767441987991333</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1935,13 +2058,16 @@
         <v>0.57015502452850342</v>
       </c>
       <c r="E12">
+        <v>0.57984495162963867</v>
+      </c>
+      <c r="F12">
         <v>0.59573644399642944</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>0.60116279125213623</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1955,13 +2081,16 @@
         <v>0.56627905368804932</v>
       </c>
       <c r="E13">
+        <v>0.60348838567733765</v>
+      </c>
+      <c r="F13">
         <v>0.59922480583190918</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>0.59534883499145508</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1975,13 +2104,16 @@
         <v>0.57480621337890625</v>
       </c>
       <c r="E14">
+        <v>0.60348838567733765</v>
+      </c>
+      <c r="F14">
         <v>0.59069764614105225</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>0.59457361698150635</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1995,13 +2127,16 @@
         <v>0.57519382238388062</v>
       </c>
       <c r="E15">
+        <v>0.60736435651779175</v>
+      </c>
+      <c r="F15">
         <v>0.58682173490524292</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>0.60581398010253906</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2015,10 +2150,38 @@
         <v>0.56046509742736816</v>
       </c>
       <c r="E16">
+        <v>0.6003875732421875</v>
+      </c>
+      <c r="F16">
         <v>0.59108525514602661</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>0.61356586217880249</v>
+      </c>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>0.6290697455406189</v>
+      </c>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>0.60736435651779175</v>
+      </c>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <v>0.63914728164672852</v>
+      </c>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <v>0.61279070377349854</v>
+      </c>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <v>0.59147286415100098</v>
       </c>
     </row>
   </sheetData>

</xml_diff>